<commit_message>
Cambios 17 de junio:
</commit_message>
<xml_diff>
--- a/Interfaz/participantes.xlsx
+++ b/Interfaz/participantes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -487,11 +487,11 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Montaña.mp4</t>
+          <t>Costa.mp4</t>
         </is>
       </c>
     </row>
@@ -505,6 +505,21 @@
         <v>18</v>
       </c>
       <c r="C5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>DS3</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Costa.mp4</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>